<commit_message>
run: with adjusted supply side/IRA forecast
Replace old CORRECTED CBO + SUPPLY SIDE folder with new one
</commit_message>
<xml_diff>
--- a/results/05-2024 - CORRECTED CBO + SUPPLY SIDE/comparison-deflators-05-2024.xlsx
+++ b/results/05-2024 - CORRECTED CBO + SUPPLY SIDE/comparison-deflators-05-2024.xlsx
@@ -883,52 +883,52 @@
         <v>-0.0708</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0969</v>
+        <v>0.1067</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.045</v>
+        <v>-0.0452</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2751</v>
+        <v>0.295</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2384</v>
+        <v>0.2573</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5026</v>
+        <v>0.3088</v>
       </c>
       <c r="M6" t="n">
-        <v>0.5367</v>
+        <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7111</v>
+        <v>0.1561</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3556</v>
+        <v>-0.0145</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1834</v>
+        <v>-0.0203</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1366</v>
+        <v>-0.0138</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0037</v>
+        <v>-0.0083</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0363</v>
+        <v>0.0126</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0316</v>
+        <v>0.0046</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0962</v>
+        <v>-0.005</v>
       </c>
       <c r="V6" t="n">
-        <v>0.122</v>
+        <v>-0.0105</v>
       </c>
       <c r="W6" t="n">
-        <v>-3.7756</v>
+        <v>-1.7941</v>
       </c>
     </row>
     <row r="7">
@@ -1593,52 +1593,52 @@
         <v>-4.5905</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.2972</v>
+        <v>-2.2874</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.5605</v>
+        <v>-0.5607</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0439</v>
+        <v>0.0638</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.2074</v>
+        <v>-0.1884</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7225</v>
+        <v>0.5287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4883</v>
+        <v>0.2312</v>
       </c>
       <c r="N16" t="n">
-        <v>0.3005</v>
+        <v>-0.2545</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.2837</v>
+        <v>-0.6538</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.0332</v>
+        <v>-0.2369</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1419</v>
+        <v>-0.0086</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.5106</v>
+        <v>-0.5226</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.6713</v>
+        <v>-0.6951</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.4579</v>
+        <v>-0.4849</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.3235</v>
+        <v>-0.4247</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0767</v>
+        <v>-0.0558</v>
       </c>
       <c r="W16" t="n">
-        <v>-75.1223</v>
+        <v>-73.1408</v>
       </c>
     </row>
     <row r="17">
@@ -2871,52 +2871,52 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.0098</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.0199</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.019</v>
+        <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1938</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.2571</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>0.555</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>0.4759</v>
+        <v>0.1058</v>
       </c>
       <c r="P34" t="n">
-        <v>0.4215</v>
+        <v>0.2178</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.3602</v>
+        <v>0.2097</v>
       </c>
       <c r="R34" t="n">
-        <v>0.2876</v>
+        <v>0.2755</v>
       </c>
       <c r="S34" t="n">
-        <v>0.2558</v>
+        <v>0.2321</v>
       </c>
       <c r="T34" t="n">
-        <v>0.2023</v>
+        <v>0.1752</v>
       </c>
       <c r="U34" t="n">
-        <v>0.1317</v>
+        <v>0.0305</v>
       </c>
       <c r="V34" t="n">
-        <v>0.2361</v>
+        <v>0.1036</v>
       </c>
       <c r="W34" t="n">
-        <v>-3.3484</v>
+        <v>-1.3669</v>
       </c>
     </row>
     <row r="35">
@@ -3581,52 +3581,52 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.0098</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.0199</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.019</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.1938</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.2571</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0.555</v>
+        <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>0.3901</v>
+        <v>0.02</v>
       </c>
       <c r="P44" t="n">
-        <v>0.3298</v>
+        <v>0.1261</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.2609</v>
+        <v>0.1105</v>
       </c>
       <c r="R44" t="n">
-        <v>0.1757</v>
+        <v>0.1636</v>
       </c>
       <c r="S44" t="n">
-        <v>0.1482</v>
+        <v>0.1244</v>
       </c>
       <c r="T44" t="n">
-        <v>0.1063</v>
+        <v>0.0793</v>
       </c>
       <c r="U44" t="n">
-        <v>0.0469</v>
+        <v>-0.0543</v>
       </c>
       <c r="V44" t="n">
-        <v>0.1676</v>
+        <v>0.0352</v>
       </c>
       <c r="W44" t="n">
-        <v>-4.4752</v>
+        <v>-2.4937</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
Merge 'results/05-2024 - CORRECTED CBO + SUPPLY SIDE' directory into refactor/collect-data
</commit_message>
<xml_diff>
--- a/results/05-2024 - CORRECTED CBO + SUPPLY SIDE/comparison-deflators-05-2024.xlsx
+++ b/results/05-2024 - CORRECTED CBO + SUPPLY SIDE/comparison-deflators-05-2024.xlsx
@@ -883,52 +883,52 @@
         <v>-0.0708</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0969</v>
+        <v>0.1067</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.045</v>
+        <v>-0.0452</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2751</v>
+        <v>0.295</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2384</v>
+        <v>0.2573</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5026</v>
+        <v>0.3088</v>
       </c>
       <c r="M6" t="n">
-        <v>0.5367</v>
+        <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7111</v>
+        <v>0.1561</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3556</v>
+        <v>-0.0145</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1834</v>
+        <v>-0.0203</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1366</v>
+        <v>-0.0138</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0037</v>
+        <v>-0.0083</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0363</v>
+        <v>0.0126</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0316</v>
+        <v>0.0046</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0962</v>
+        <v>-0.005</v>
       </c>
       <c r="V6" t="n">
-        <v>0.122</v>
+        <v>-0.0105</v>
       </c>
       <c r="W6" t="n">
-        <v>-3.7756</v>
+        <v>-1.7941</v>
       </c>
     </row>
     <row r="7">
@@ -1593,52 +1593,52 @@
         <v>-4.5905</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.2972</v>
+        <v>-2.2874</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.5605</v>
+        <v>-0.5607</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0439</v>
+        <v>0.0638</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.2074</v>
+        <v>-0.1884</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7225</v>
+        <v>0.5287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4883</v>
+        <v>0.2312</v>
       </c>
       <c r="N16" t="n">
-        <v>0.3005</v>
+        <v>-0.2545</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.2837</v>
+        <v>-0.6538</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.0332</v>
+        <v>-0.2369</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1419</v>
+        <v>-0.0086</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.5106</v>
+        <v>-0.5226</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.6713</v>
+        <v>-0.6951</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.4579</v>
+        <v>-0.4849</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.3235</v>
+        <v>-0.4247</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0767</v>
+        <v>-0.0558</v>
       </c>
       <c r="W16" t="n">
-        <v>-75.1223</v>
+        <v>-73.1408</v>
       </c>
     </row>
     <row r="17">
@@ -2871,52 +2871,52 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.0098</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.0199</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.019</v>
+        <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1938</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.2571</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>0.555</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>0.4759</v>
+        <v>0.1058</v>
       </c>
       <c r="P34" t="n">
-        <v>0.4215</v>
+        <v>0.2178</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.3602</v>
+        <v>0.2097</v>
       </c>
       <c r="R34" t="n">
-        <v>0.2876</v>
+        <v>0.2755</v>
       </c>
       <c r="S34" t="n">
-        <v>0.2558</v>
+        <v>0.2321</v>
       </c>
       <c r="T34" t="n">
-        <v>0.2023</v>
+        <v>0.1752</v>
       </c>
       <c r="U34" t="n">
-        <v>0.1317</v>
+        <v>0.0305</v>
       </c>
       <c r="V34" t="n">
-        <v>0.2361</v>
+        <v>0.1036</v>
       </c>
       <c r="W34" t="n">
-        <v>-3.3484</v>
+        <v>-1.3669</v>
       </c>
     </row>
     <row r="35">
@@ -3581,52 +3581,52 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.0098</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.0199</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.019</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.1938</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.2571</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0.555</v>
+        <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>0.3901</v>
+        <v>0.02</v>
       </c>
       <c r="P44" t="n">
-        <v>0.3298</v>
+        <v>0.1261</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.2609</v>
+        <v>0.1105</v>
       </c>
       <c r="R44" t="n">
-        <v>0.1757</v>
+        <v>0.1636</v>
       </c>
       <c r="S44" t="n">
-        <v>0.1482</v>
+        <v>0.1244</v>
       </c>
       <c r="T44" t="n">
-        <v>0.1063</v>
+        <v>0.0793</v>
       </c>
       <c r="U44" t="n">
-        <v>0.0469</v>
+        <v>-0.0543</v>
       </c>
       <c r="V44" t="n">
-        <v>0.1676</v>
+        <v>0.0352</v>
       </c>
       <c r="W44" t="n">
-        <v>-4.4752</v>
+        <v>-2.4937</v>
       </c>
     </row>
     <row r="45">

</xml_diff>